<commit_message>
node switchup and more predictions
</commit_message>
<xml_diff>
--- a/Data/Compute/scf_cpus.xlsx
+++ b/Data/Compute/scf_cpus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\computer-vision-project\Data\Compute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67074F1A-33EC-4AD9-8D05-ABF921450ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5220A1-8A0A-45D8-870C-648098922870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{86A1FC72-5D68-4751-A2DE-A2B260FE0B28}"/>
+    <workbookView xWindow="444" yWindow="2760" windowWidth="17280" windowHeight="8892" xr2:uid="{86A1FC72-5D68-4751-A2DE-A2B260FE0B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>partition</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Intel Xeon Gold 5218 CPU @ 2.30GHz</t>
+  </si>
+  <si>
+    <t>samwise</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEC221D-E1F4-4746-98CC-7563091684FA}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +590,20 @@
         <v>21986</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>60132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>